<commit_message>
Planilha de organização task 05
</commit_message>
<xml_diff>
--- a/Planilha_organizacao_tarefas_2021.xlsx
+++ b/Planilha_organizacao_tarefas_2021.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
   <si>
     <t>DISTRIBUIÇÃO DAS TAREFAS – PROJETO INTEGRADOR</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>TASK 07</t>
+  </si>
+  <si>
+    <t>Gabriel Maia</t>
   </si>
   <si>
     <t>TASK 08</t>
@@ -376,7 +379,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -488,7 +491,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -600,7 +603,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -712,7 +715,7 @@
     <xdr:ext cx="438150" cy="885825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -824,7 +827,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -908,7 +911,7 @@
     <xdr:ext cx="1285875" cy="533400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Texto&#10;&#10;Descrição gerada automaticamente com confiança média" id="0" name="image2.png"/>
+        <xdr:cNvPr descr="Texto&#10;&#10;Descrição gerada automaticamente com confiança média" id="0" name="image5.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -964,7 +967,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1076,7 +1079,7 @@
     <xdr:ext cx="438150" cy="885825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1193,7 +1196,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1305,7 +1308,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1417,7 +1420,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1529,7 +1532,7 @@
     <xdr:ext cx="438150" cy="885825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1641,7 +1644,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1725,7 +1728,7 @@
     <xdr:ext cx="1285875" cy="533400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Texto&#10;&#10;Descrição gerada automaticamente com confiança média" id="0" name="image2.png"/>
+        <xdr:cNvPr descr="Texto&#10;&#10;Descrição gerada automaticamente com confiança média" id="0" name="image5.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1781,7 +1784,7 @@
     <xdr:ext cx="438150" cy="885825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1893,7 +1896,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2005,7 +2008,7 @@
     <xdr:ext cx="438150" cy="895350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Diagrama&#10;&#10;Descrição gerada automaticamente com confiança baixa" id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2654,7 +2657,9 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
+      <c r="B26" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="C26" s="13"/>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
@@ -2694,7 +2699,9 @@
     </row>
     <row r="30" ht="20.25" customHeight="1">
       <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
+      <c r="B30" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
       <c r="G30" s="11"/>
@@ -2726,7 +2733,9 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
-      <c r="B34" s="18"/>
+      <c r="B34" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="D34" s="17"/>
       <c r="E34" s="18"/>
       <c r="G34" s="17"/>
@@ -2734,7 +2743,9 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="20"/>
-      <c r="B35" s="18"/>
+      <c r="B35" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="D35" s="20"/>
       <c r="E35" s="18"/>
       <c r="G35" s="20"/>
@@ -2742,7 +2753,9 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="20"/>
-      <c r="B36" s="18"/>
+      <c r="B36" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="D36" s="20"/>
       <c r="E36" s="18"/>
       <c r="G36" s="20"/>
@@ -2750,7 +2763,9 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="21"/>
-      <c r="B37" s="22"/>
+      <c r="B37" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="G37" s="21"/>
@@ -2758,7 +2773,9 @@
     </row>
     <row r="38" ht="20.25" customHeight="1">
       <c r="A38" s="11"/>
-      <c r="B38" s="12"/>
+      <c r="B38" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="D38" s="11"/>
       <c r="E38" s="12"/>
       <c r="G38" s="11"/>
@@ -2795,7 +2812,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B43" s="8"/>
       <c r="E43" s="5"/>
@@ -8077,15 +8094,15 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8"/>
       <c r="D5" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="8"/>
       <c r="G5" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" s="8"/>
     </row>
@@ -8324,15 +8341,15 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" s="8"/>
       <c r="D24" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E24" s="8"/>
       <c r="G24" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H24" s="8"/>
     </row>
@@ -8499,11 +8516,11 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B43" s="8"/>
       <c r="D43" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E43" s="8"/>
       <c r="H43" s="5"/>

</xml_diff>